<commit_message>
added mouseover function to each state
</commit_message>
<xml_diff>
--- a/data/variable definitions.xlsx
+++ b/data/variable definitions.xlsx
@@ -310,10 +310,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,28 +593,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44.6640625" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" customWidth="1"/>
     <col min="4" max="4" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -950,14 +950,14 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="D28" s="2" t="s">
+      <c r="B28" s="4"/>
+      <c r="D28" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
@@ -975,17 +975,17 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>